<commit_message>
cols renamed by: https://github.com/imahdimir/i-md-fundtype-portfo-compose-on-agg
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -436,14 +436,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>FundType</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>JMonth</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>FundType</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Stocks &amp; Preffered Shares</t>
@@ -471,12 +471,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>139601</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-01</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -496,12 +498,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>139601</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-01</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -521,12 +525,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>139601</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-01</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -546,12 +552,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>139601</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">کل </t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">کل </t>
+          <t>1396-01</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -571,12 +579,14 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>139602</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-02</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -596,12 +606,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>139602</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-02</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -621,12 +633,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>139602</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-02</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -646,12 +660,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>139602</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-02</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -671,12 +687,14 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>139603</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-03</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -696,12 +714,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>139603</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-03</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -721,12 +741,14 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>139603</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-03</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -746,12 +768,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>139603</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-03</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -771,12 +795,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>139604</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-04</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -796,12 +822,14 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>139604</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-04</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -821,12 +849,14 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>139604</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-04</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -846,12 +876,14 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>139604</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-04</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -871,12 +903,14 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>139605</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-05</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -896,12 +930,14 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>139605</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-05</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -921,12 +957,14 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>139605</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-05</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -946,12 +984,14 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>139605</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-05</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -971,12 +1011,14 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>139605</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-05</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -996,12 +1038,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>139606</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-06</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1021,12 +1065,14 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>139606</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-06</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1046,12 +1092,14 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>139606</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-06</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1071,12 +1119,14 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>139606</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-06</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1096,12 +1146,14 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>139606</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-06</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1121,12 +1173,14 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>139607</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-07</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1146,12 +1200,14 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>139607</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-07</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1171,12 +1227,14 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>139607</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-07</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1196,12 +1254,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>139607</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-07</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1221,12 +1281,14 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>139607</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-07</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1246,12 +1308,14 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>139608</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-08</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1271,12 +1335,14 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>139608</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-08</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1296,12 +1362,14 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>139608</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-08</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1321,12 +1389,14 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>139608</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-08</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1346,12 +1416,14 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>139608</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-08</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1371,12 +1443,14 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>139609</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-09</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1396,12 +1470,14 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>139609</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-09</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1421,12 +1497,14 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>139609</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-09</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1446,12 +1524,14 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>139609</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-09</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1471,12 +1551,14 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>139609</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-09</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1496,12 +1578,14 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>139610</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-10</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1521,12 +1605,14 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>139610</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-10</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1546,12 +1632,14 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>139610</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-10</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1571,12 +1659,14 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>139610</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-10</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1596,12 +1686,14 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>139610</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-10</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1621,12 +1713,14 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>139611</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-11</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1646,12 +1740,14 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>139611</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-11</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1671,12 +1767,14 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>139611</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-11</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1696,12 +1794,14 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>139611</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-11</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1721,12 +1821,14 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>139611</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-11</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1746,12 +1848,14 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>139612</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1396-12</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1771,12 +1875,14 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>139612</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1396-12</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1796,12 +1902,14 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>139612</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1396-12</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1821,12 +1929,14 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>139612</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1396-12</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1846,12 +1956,14 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>139612</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1396-12</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1871,12 +1983,14 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>139701</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-01</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1896,12 +2010,14 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>139701</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-01</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1921,12 +2037,14 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>139701</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-01</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1946,12 +2064,14 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>139701</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-01</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1971,12 +2091,14 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>139701</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-01</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1996,12 +2118,14 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>139702</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-02</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -2021,12 +2145,14 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>139702</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-02</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2046,12 +2172,14 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>139702</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-02</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -2071,12 +2199,14 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>139702</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-02</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -2096,12 +2226,14 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>139702</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-02</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -2121,12 +2253,14 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>139703</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-03</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -2146,12 +2280,14 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>139703</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-03</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -2171,12 +2307,14 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>139703</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-03</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2196,12 +2334,14 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>139703</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-03</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2221,12 +2361,14 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>139703</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-03</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2246,12 +2388,14 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>139704</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-04</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -2271,12 +2415,14 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>139704</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-04</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -2296,12 +2442,14 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>139704</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-04</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -2321,12 +2469,14 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>139704</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-04</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2346,12 +2496,14 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>139704</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-04</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2371,12 +2523,14 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>139705</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-05</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2396,12 +2550,14 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>139705</v>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-05</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2421,12 +2577,14 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>139705</v>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-05</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2446,12 +2604,14 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>139705</v>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-05</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2471,12 +2631,14 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>139705</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-05</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2496,12 +2658,14 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>139706</v>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-06</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2521,12 +2685,14 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>139706</v>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-06</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2546,12 +2712,14 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>139706</v>
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-06</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -2571,12 +2739,14 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>139706</v>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-06</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -2596,12 +2766,14 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>139706</v>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-06</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2621,12 +2793,14 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>139707</v>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-07</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -2646,12 +2820,14 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>139707</v>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-07</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -2671,12 +2847,14 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>139707</v>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-07</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2696,12 +2874,14 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>139707</v>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-07</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2721,12 +2901,14 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>139707</v>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-07</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2746,12 +2928,14 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>139708</v>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-08</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2771,12 +2955,14 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>139708</v>
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-08</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -2796,12 +2982,14 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>139708</v>
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-08</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2821,12 +3009,14 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
-        <v>139708</v>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-08</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -2846,12 +3036,14 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
-        <v>139708</v>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-08</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2871,12 +3063,14 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
-        <v>139709</v>
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-09</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2896,12 +3090,14 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>139709</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-09</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2921,12 +3117,14 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
-        <v>139709</v>
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-09</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2946,12 +3144,14 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
-        <v>139709</v>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-09</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2971,12 +3171,14 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
-        <v>139709</v>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-09</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2996,12 +3198,14 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
-        <v>139710</v>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-10</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -3021,12 +3225,14 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
-        <v>139710</v>
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-10</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -3046,12 +3252,14 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
-        <v>139710</v>
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-10</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -3071,12 +3279,14 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
-        <v>139710</v>
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-10</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -3096,12 +3306,14 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
-        <v>139710</v>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-10</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -3121,12 +3333,14 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
-        <v>139711</v>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-11</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3146,12 +3360,14 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
-        <v>139711</v>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-11</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -3171,12 +3387,14 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
-        <v>139711</v>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-11</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -3196,12 +3414,14 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
-        <v>139711</v>
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-11</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -3221,12 +3441,14 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="n">
-        <v>139711</v>
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-11</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -3246,12 +3468,14 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="n">
-        <v>139712</v>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1397-12</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -3271,12 +3495,14 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="n">
-        <v>139712</v>
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1397-12</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -3296,12 +3522,14 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="n">
-        <v>139712</v>
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1397-12</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -3321,12 +3549,14 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="n">
-        <v>139712</v>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1397-12</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -3346,12 +3576,14 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n">
-        <v>139712</v>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1397-12</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3371,12 +3603,14 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n">
-        <v>139801</v>
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-01</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -3396,12 +3630,14 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n">
-        <v>139801</v>
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-01</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -3421,12 +3657,14 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="n">
-        <v>139801</v>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-01</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -3446,12 +3684,14 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="n">
-        <v>139801</v>
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-01</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -3471,12 +3711,14 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="n">
-        <v>139801</v>
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-01</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -3496,12 +3738,14 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="n">
-        <v>139802</v>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-02</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -3521,12 +3765,14 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="n">
-        <v>139802</v>
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-02</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -3546,12 +3792,14 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="n">
-        <v>139802</v>
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-02</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -3571,12 +3819,14 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="n">
-        <v>139802</v>
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-02</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -3596,12 +3846,14 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="n">
-        <v>139802</v>
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-02</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -3621,12 +3873,14 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="n">
-        <v>139803</v>
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-03</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -3646,12 +3900,14 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="n">
-        <v>139803</v>
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-03</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -3671,12 +3927,14 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
-        <v>139803</v>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-03</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -3696,12 +3954,14 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
-        <v>139803</v>
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-03</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -3721,12 +3981,14 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
-        <v>139803</v>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-03</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -3746,12 +4008,14 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
-        <v>139804</v>
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-04</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -3771,12 +4035,14 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="n">
-        <v>139804</v>
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-04</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -3796,12 +4062,14 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="n">
-        <v>139804</v>
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-04</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -3821,12 +4089,14 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="n">
-        <v>139804</v>
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-04</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -3846,12 +4116,14 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="n">
-        <v>139804</v>
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-04</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -3871,12 +4143,14 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="n">
-        <v>139805</v>
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-05</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -3896,12 +4170,14 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="n">
-        <v>139805</v>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-05</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -3921,12 +4197,14 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="n">
-        <v>139805</v>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-05</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -3946,12 +4224,14 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="n">
-        <v>139805</v>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-05</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -3971,12 +4251,14 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="n">
-        <v>139805</v>
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-05</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -3996,12 +4278,14 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="n">
-        <v>139806</v>
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-06</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -4021,12 +4305,14 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="n">
-        <v>139806</v>
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-06</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -4046,12 +4332,14 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="n">
-        <v>139806</v>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-06</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -4071,12 +4359,14 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="n">
-        <v>139806</v>
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-06</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -4096,12 +4386,14 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="n">
-        <v>139806</v>
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-06</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -4121,12 +4413,14 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="n">
-        <v>139807</v>
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-07</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -4146,12 +4440,14 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="n">
-        <v>139807</v>
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-07</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -4171,12 +4467,14 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="n">
-        <v>139807</v>
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-07</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -4196,12 +4494,14 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="n">
-        <v>139807</v>
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-07</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -4221,12 +4521,14 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="n">
-        <v>139807</v>
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-07</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -4246,12 +4548,14 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="n">
-        <v>139808</v>
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-08</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -4271,12 +4575,14 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="n">
-        <v>139808</v>
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-08</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -4296,12 +4602,14 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="n">
-        <v>139808</v>
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-08</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -4321,12 +4629,14 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="n">
-        <v>139808</v>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>اختصاصی بازارگردانی</t>
+        </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی</t>
+          <t>1398-08</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -4346,12 +4656,14 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="n">
-        <v>139808</v>
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-08</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -4371,12 +4683,14 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="n">
-        <v>139809</v>
+      <c r="A158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوراق بهادار با درآمد ثابت </t>
+        </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t xml:space="preserve">اوراق بهادار با درآمد ثابت </t>
+          <t>1398-09</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -4396,12 +4710,14 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="n">
-        <v>139809</v>
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-09</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -4421,12 +4737,14 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="n">
-        <v>139809</v>
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-09</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -4446,12 +4764,14 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="n">
-        <v>139809</v>
+      <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1398-09</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -4471,12 +4791,14 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="n">
-        <v>139809</v>
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-09</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -4496,12 +4818,14 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="n">
-        <v>139810</v>
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-10</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -4521,12 +4845,14 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="n">
-        <v>139810</v>
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-10</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -4546,12 +4872,14 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="n">
-        <v>139810</v>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-10</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -4571,12 +4899,14 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="n">
-        <v>139810</v>
+      <c r="A166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1398-10</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -4596,12 +4926,14 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="n">
-        <v>139810</v>
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-10</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -4621,12 +4953,14 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="n">
-        <v>139811</v>
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-11</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -4646,12 +4980,14 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="n">
-        <v>139811</v>
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-11</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -4671,12 +5007,14 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="n">
-        <v>139811</v>
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-11</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -4696,12 +5034,14 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="n">
-        <v>139811</v>
+      <c r="A171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1398-11</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -4721,12 +5061,14 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="n">
-        <v>139811</v>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-11</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -4746,12 +5088,14 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="n">
-        <v>139812</v>
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1398-12</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -4771,12 +5115,14 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="n">
-        <v>139812</v>
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1398-12</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -4796,12 +5142,14 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
-        <v>139812</v>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1398-12</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -4821,12 +5169,14 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
-        <v>139812</v>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1398-12</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -4846,12 +5196,14 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="n">
-        <v>139812</v>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1398-12</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -4871,12 +5223,14 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="n">
-        <v>139901</v>
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-01</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -4896,12 +5250,14 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="n">
-        <v>139901</v>
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-01</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -4921,12 +5277,14 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="n">
-        <v>139901</v>
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-01</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -4946,12 +5304,14 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="n">
-        <v>139901</v>
+      <c r="A181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-01</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -4971,12 +5331,14 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="n">
-        <v>139901</v>
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-01</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -4996,12 +5358,14 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="n">
-        <v>139902</v>
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-02</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -5021,12 +5385,14 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="n">
-        <v>139902</v>
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-02</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -5046,12 +5412,14 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="n">
-        <v>139902</v>
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-02</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -5071,12 +5439,14 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="n">
-        <v>139902</v>
+      <c r="A186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-02</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -5096,12 +5466,14 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="n">
-        <v>139902</v>
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-02</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -5121,12 +5493,14 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="n">
-        <v>139903</v>
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-03</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -5146,12 +5520,14 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="n">
-        <v>139903</v>
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-03</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -5171,12 +5547,14 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="n">
-        <v>139903</v>
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-03</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -5196,12 +5574,14 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="n">
-        <v>139903</v>
+      <c r="A191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-03</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -5221,12 +5601,14 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="n">
-        <v>139903</v>
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-03</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -5246,12 +5628,14 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="n">
-        <v>139904</v>
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-04</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -5271,12 +5655,14 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="n">
-        <v>139904</v>
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-04</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -5296,12 +5682,14 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="n">
-        <v>139904</v>
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-04</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -5321,12 +5709,14 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="n">
-        <v>139904</v>
+      <c r="A196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-04</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -5346,12 +5736,14 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="n">
-        <v>139904</v>
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-04</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -5371,12 +5763,14 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="n">
-        <v>139905</v>
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-05</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -5396,12 +5790,14 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="n">
-        <v>139905</v>
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-05</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -5421,12 +5817,14 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="n">
-        <v>139905</v>
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-05</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -5446,12 +5844,14 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="n">
-        <v>139905</v>
+      <c r="A201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-05</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -5471,12 +5871,14 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="n">
-        <v>139905</v>
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-05</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -5496,12 +5898,14 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="n">
-        <v>139906</v>
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-06</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -5521,12 +5925,14 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="n">
-        <v>139906</v>
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-06</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -5546,12 +5952,14 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="n">
-        <v>139906</v>
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-06</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -5571,12 +5979,14 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="n">
-        <v>139906</v>
+      <c r="A206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-06</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -5596,12 +6006,14 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="n">
-        <v>139906</v>
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-06</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -5621,12 +6033,14 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="n">
-        <v>139907</v>
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>اوراق بهادار با درآمد ثابت</t>
+        </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>اوراق بهادار با درآمد ثابت</t>
+          <t>1399-07</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -5646,12 +6060,14 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" t="n">
-        <v>139907</v>
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>مختلط</t>
+        </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>مختلط</t>
+          <t>1399-07</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -5671,12 +6087,14 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" t="n">
-        <v>139907</v>
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>سهام</t>
+        </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>سهام</t>
+          <t>1399-07</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -5696,12 +6114,14 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" t="n">
-        <v>139907</v>
+      <c r="A211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+        </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t xml:space="preserve">اختصاصی بازارگردانی </t>
+          <t>1399-07</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -5721,12 +6141,14 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="n">
-        <v>139907</v>
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>کل</t>
+        </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>کل</t>
+          <t>1399-07</t>
         </is>
       </c>
       <c r="C212" t="n">

</xml_diff>